<commit_message>
much faster processing time for model
</commit_message>
<xml_diff>
--- a/bill_of_materials.xlsx
+++ b/bill_of_materials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://1sfu-my.sharepoint.com/personal/rcalara_sfu_ca/Documents/SFU/SFU Classes/MSE312/project/matlab_and_solidworks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://1sfu-my.sharepoint.com/personal/rcalara_sfu_ca/Documents/SFU/SFU Classes/MSE312/project/mse312_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="11_F25DC773A252ABDACC104815A15B7F005ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1043BBE4-72BC-44D0-BC11-ADA83D4B8741}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="11_F25DC773A252ABDACC104815A15B7F005ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1348B925-5A82-439E-9E15-8C4A3340773C}"/>
   <bookViews>
-    <workbookView xWindow="11730" yWindow="4200" windowWidth="13620" windowHeight="9315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9945" yWindow="3885" windowWidth="13620" windowHeight="9315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,18 +51,9 @@
     <t>https://www.grainger.ca/en/product/FLAT-STOCK%2CAL%2C6061%2C1-X-4-IN%2C1-FT/p/WWG2EZW6</t>
   </si>
   <si>
-    <t>Cytron 25A 7-58V Single Brushed DC Motor Driver</t>
-  </si>
-  <si>
     <t>https://www.robotshop.com/ca/en/cytron-25a-7-58v-single-brushed-dc-motor-driver.html</t>
   </si>
   <si>
-    <t>AmpFlow E30-400-24 High-Performance Motor 12-48VDC 5700 RPM</t>
-  </si>
-  <si>
-    <t>https://www.robotshop.com/ca/en/ampflow-e30-400-24-high-performance-motor-12-48vdc-5700-rpm.html?gclid=CjwKCAjwrPCGBhALEiwAUl9X01LieUFVC5H1OU3DkIGtJUrEvh7uF6IssY9LOVLmNshTB6yP8MiiOxoC0SEQAvD_BwE</t>
-  </si>
-  <si>
     <t>Arm (PET) 100% fill</t>
   </si>
   <si>
@@ -91,6 +82,15 @@
   </si>
   <si>
     <t>3/8" Diameter shaft, 12" length</t>
+  </si>
+  <si>
+    <t>H-Bridge Driver 24V 8A</t>
+  </si>
+  <si>
+    <t>Crouzet 82890001</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/crouzet/82890001/3190319</t>
   </si>
 </sst>
 </file>
@@ -422,7 +422,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,85 +454,85 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3">
-        <v>62.82</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B4">
-        <v>155.71</v>
+        <v>311.60000000000002</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>71.72</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>9.86</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>56.68</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>19.71</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10">
         <f>SUM(B2:B9)</f>
-        <v>465.65999999999997</v>
+        <v>600.73</v>
       </c>
     </row>
   </sheetData>
@@ -540,5 +540,6 @@
     <hyperlink ref="C7" r:id="rId1" xr:uid="{23954ECB-1E10-4CEE-97E3-570DE6DC3F4A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>